<commit_message>
"Testing One zipcode data for 4k Categories"
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,17 +387,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>335</v>
+        <v>201301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Complete flow for one zipcode"
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +387,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>201301</v>
+        <v>201302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>